<commit_message>
update main flow. read files in folder and pass to process.xaml
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Automation\RS-Vendors\HOS-Invoice-Loading-Dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\rpabots_ws\HOS-Invoice-Loading-Dispatcjer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC63764-8B74-4CEA-BBA6-357A6B38532C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF273113-7C59-4BE3-AAC8-9E127CCD0162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1695,7 +1695,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>